<commit_message>
data loaded, def functions for vector add, sub, mult, div and created data_btm
</commit_message>
<xml_diff>
--- a/03_CarryTask/02_Data_clean/SPX_Value_clean.xlsx
+++ b/03_CarryTask/02_Data_clean/SPX_Value_clean.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Dropbox/00 UZH/Master/PMP/01. Offline PMP/PMP Coding/Vitznau/03_CarryTask/02_Data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA98DD81-C93B-5847-A971-3CC4A6FCF685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E95963A-29CD-CB41-A416-ACF9A0332464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28700" windowHeight="11680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1546,10 +1546,10 @@
     <t>CMCSK UQ Equity</t>
   </si>
   <si>
-    <t>Dates</t>
-  </si>
-  <si>
     <t>#N/A N/A</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -1870,7 +1870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:SG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1879,7 +1881,7 @@
   <sheetData>
     <row r="1" spans="1:501" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3393,13 +3395,13 @@
         <v>12.501799999999999</v>
       </c>
       <c r="D2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E2">
         <v>12.303699999999999</v>
       </c>
       <c r="F2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G2">
         <v>10.4899</v>
@@ -3486,7 +3488,7 @@
         <v>2.4438</v>
       </c>
       <c r="AI2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AJ2">
         <v>11.1686</v>
@@ -3699,7 +3701,7 @@
         <v>4.3213999999999997</v>
       </c>
       <c r="DB2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="DC2">
         <v>3.5087999999999999</v>
@@ -4068,10 +4070,10 @@
         <v>7.1087999999999996</v>
       </c>
       <c r="HU2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="HV2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="HW2">
         <v>10.7119</v>
@@ -4080,7 +4082,7 @@
         <v>20.4024</v>
       </c>
       <c r="HY2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="HZ2">
         <v>16.8536</v>
@@ -4173,7 +4175,7 @@
         <v>3.9737</v>
       </c>
       <c r="JD2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="JE2">
         <v>7.8902000000000001</v>
@@ -4314,7 +4316,7 @@
         <v>7.2979000000000003</v>
       </c>
       <c r="KY2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="KZ2">
         <v>5.8333000000000004</v>
@@ -4434,7 +4436,7 @@
         <v>92.279300000000006</v>
       </c>
       <c r="MM2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN2">
         <v>5.9394</v>
@@ -4692,7 +4694,7 @@
         <v>74.925200000000004</v>
       </c>
       <c r="PU2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="PV2">
         <v>16.7807</v>
@@ -4746,7 +4748,7 @@
         <v>24.765999999999998</v>
       </c>
       <c r="QM2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="QN2">
         <v>5.2401999999999997</v>
@@ -4878,7 +4880,7 @@
         <v>1.4718</v>
       </c>
       <c r="SE2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="SF2">
         <v>19.411200000000001</v>
@@ -4985,7 +4987,7 @@
         <v>3.3178999999999998</v>
       </c>
       <c r="AI3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AJ3">
         <v>11.1686</v>
@@ -5891,7 +5893,7 @@
         <v>84.702699999999993</v>
       </c>
       <c r="MM3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN3">
         <v>7.3170000000000002</v>
@@ -6149,7 +6151,7 @@
         <v>74.925200000000004</v>
       </c>
       <c r="PU3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="PW3">
         <v>16.540500000000002</v>
@@ -6421,7 +6423,7 @@
         <v>3.7233999999999998</v>
       </c>
       <c r="AI4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AJ4">
         <v>18.428599999999999</v>
@@ -7300,7 +7302,7 @@
         <v>1.851</v>
       </c>
       <c r="MM4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN4">
         <v>10.979799999999999</v>
@@ -7546,7 +7548,7 @@
         <v>74.925200000000004</v>
       </c>
       <c r="PU4" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="PW4">
         <v>16.540500000000002</v>
@@ -7815,7 +7817,7 @@
         <v>3.1208999999999998</v>
       </c>
       <c r="AI5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AJ5">
         <v>15.8794</v>
@@ -8679,7 +8681,7 @@
         <v>-191.5401</v>
       </c>
       <c r="MM5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN5">
         <v>9.9507999999999992</v>
@@ -8916,7 +8918,7 @@
         <v>7.4954000000000001</v>
       </c>
       <c r="PU5" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="PW5">
         <v>16.540500000000002</v>
@@ -9185,7 +9187,7 @@
         <v>2.7608000000000001</v>
       </c>
       <c r="AI6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="AJ6">
         <v>17.3032</v>
@@ -10031,7 +10033,7 @@
         <v>-213.9802</v>
       </c>
       <c r="MM6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN6">
         <v>10.630100000000001</v>
@@ -10262,7 +10264,7 @@
         <v>8.5021000000000004</v>
       </c>
       <c r="PU6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="PW6">
         <v>16.540500000000002</v>
@@ -11359,7 +11361,7 @@
         <v>-6.4816000000000003</v>
       </c>
       <c r="MM7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN7">
         <v>11.3133</v>
@@ -12657,7 +12659,7 @@
         <v>-2.9685000000000001</v>
       </c>
       <c r="MM8" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN8">
         <v>12.685600000000001</v>
@@ -13922,7 +13924,7 @@
         <v>0.46110000000000001</v>
       </c>
       <c r="MM9" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="MN9">
         <v>12.8005</v>

</xml_diff>

<commit_message>
spx index and fed fund rate loaded but not in plot yet
</commit_message>
<xml_diff>
--- a/03_CarryTask/02_Data_clean/SPX_Value_clean.xlsx
+++ b/03_CarryTask/02_Data_clean/SPX_Value_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Dropbox/00 UZH/Master/PMP/01. Offline PMP/PMP Coding/Vitznau/03_CarryTask/02_Data_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E95963A-29CD-CB41-A416-ACF9A0332464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F5FC8E-5222-884F-A63E-F7189D84AB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28700" windowHeight="11680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39980" windowHeight="18940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Book" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="502">
   <si>
     <t>AEE UN Equity</t>
   </si>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:SG24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="RT1" workbookViewId="0">
+      <selection activeCell="SI13" sqref="SI13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5529,14 +5529,14 @@
       <c r="HH3">
         <v>6.5827</v>
       </c>
-      <c r="HI3">
-        <v>16.230799999999999</v>
+      <c r="HI3" t="s">
+        <v>500</v>
       </c>
       <c r="HJ3">
         <v>19.5776</v>
       </c>
-      <c r="HK3">
-        <v>8.2728000000000002</v>
+      <c r="HK3" t="s">
+        <v>500</v>
       </c>
       <c r="HL3">
         <v>15.6478</v>
@@ -5571,20 +5571,20 @@
       <c r="HZ3">
         <v>16.2835</v>
       </c>
-      <c r="ID3">
-        <v>24.344000000000001</v>
+      <c r="ID3" t="s">
+        <v>500</v>
       </c>
       <c r="IF3">
         <v>-25.252700000000001</v>
       </c>
-      <c r="II3">
-        <v>9.3233999999999995</v>
+      <c r="II3" t="s">
+        <v>500</v>
       </c>
       <c r="IJ3">
         <v>23.9712</v>
       </c>
-      <c r="IK3">
-        <v>11.191800000000001</v>
+      <c r="IK3" t="s">
+        <v>500</v>
       </c>
       <c r="IN3">
         <v>11.8056</v>
@@ -5733,8 +5733,8 @@
       <c r="KK3">
         <v>13.087400000000001</v>
       </c>
-      <c r="KL3">
-        <v>17.915299999999998</v>
+      <c r="KL3" t="s">
+        <v>500</v>
       </c>
       <c r="KM3">
         <v>2.1777000000000002</v>
@@ -6132,29 +6132,29 @@
       <c r="PN3">
         <v>18.299399999999999</v>
       </c>
-      <c r="PO3">
-        <v>10.150399999999999</v>
+      <c r="PO3" t="s">
+        <v>500</v>
       </c>
       <c r="PP3">
         <v>6.2920999999999996</v>
       </c>
-      <c r="PQ3">
-        <v>9.9350000000000005</v>
-      </c>
-      <c r="PR3">
-        <v>10.138999999999999</v>
+      <c r="PQ3" t="s">
+        <v>500</v>
+      </c>
+      <c r="PR3" t="s">
+        <v>500</v>
       </c>
       <c r="PS3">
         <v>21.142099999999999</v>
       </c>
-      <c r="PT3">
-        <v>74.925200000000004</v>
+      <c r="PT3" t="s">
+        <v>500</v>
       </c>
       <c r="PU3" t="s">
         <v>500</v>
       </c>
-      <c r="PW3">
-        <v>16.540500000000002</v>
+      <c r="PW3" t="s">
+        <v>500</v>
       </c>
       <c r="PX3">
         <v>18.637599999999999</v>
@@ -6174,23 +6174,26 @@
       <c r="QC3">
         <v>25.899000000000001</v>
       </c>
-      <c r="QE3">
-        <v>16.986799999999999</v>
-      </c>
-      <c r="QF3">
-        <v>10.6525</v>
-      </c>
-      <c r="QG3">
-        <v>33.804900000000004</v>
-      </c>
-      <c r="QI3">
-        <v>26.884499999999999</v>
+      <c r="QE3" t="s">
+        <v>500</v>
+      </c>
+      <c r="QF3" t="s">
+        <v>500</v>
+      </c>
+      <c r="QG3" t="s">
+        <v>500</v>
+      </c>
+      <c r="QH3" t="s">
+        <v>500</v>
+      </c>
+      <c r="QI3" t="s">
+        <v>500</v>
       </c>
       <c r="QK3">
         <v>12.2</v>
       </c>
-      <c r="QL3">
-        <v>24.765999999999998</v>
+      <c r="QL3" t="s">
+        <v>500</v>
       </c>
       <c r="QN3">
         <v>5.8688000000000002</v>
@@ -6941,26 +6944,26 @@
       <c r="GZ4">
         <v>23.383199999999999</v>
       </c>
-      <c r="HB4">
-        <v>13.764799999999999</v>
-      </c>
-      <c r="HC4">
-        <v>27.805199999999999</v>
-      </c>
-      <c r="HG4">
-        <v>2.6918000000000002</v>
-      </c>
-      <c r="HH4">
-        <v>6.5827</v>
-      </c>
-      <c r="HJ4">
-        <v>19.5776</v>
+      <c r="HB4" t="s">
+        <v>500</v>
+      </c>
+      <c r="HC4" t="s">
+        <v>500</v>
+      </c>
+      <c r="HG4" t="s">
+        <v>500</v>
+      </c>
+      <c r="HH4" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ4" t="s">
+        <v>500</v>
       </c>
       <c r="HL4">
         <v>14.516299999999999</v>
       </c>
-      <c r="HM4">
-        <v>8.2403999999999993</v>
+      <c r="HM4" t="s">
+        <v>500</v>
       </c>
       <c r="HN4">
         <v>11.8794</v>
@@ -6989,14 +6992,14 @@
       <c r="IF4">
         <v>-29.240500000000001</v>
       </c>
-      <c r="II4">
-        <v>9.3233999999999995</v>
+      <c r="II4" t="s">
+        <v>500</v>
       </c>
       <c r="IJ4">
         <v>24.151700000000002</v>
       </c>
-      <c r="IK4">
-        <v>11.191800000000001</v>
+      <c r="IK4" t="s">
+        <v>500</v>
       </c>
       <c r="IN4">
         <v>8.9763999999999999</v>
@@ -7145,8 +7148,8 @@
       <c r="KK4">
         <v>16.682500000000001</v>
       </c>
-      <c r="KL4">
-        <v>17.915299999999998</v>
+      <c r="KL4" t="s">
+        <v>500</v>
       </c>
       <c r="KM4">
         <v>3.0413999999999999</v>
@@ -7520,11 +7523,11 @@
       <c r="PG4">
         <v>6.5240999999999998</v>
       </c>
-      <c r="PH4">
-        <v>16.694400000000002</v>
-      </c>
-      <c r="PI4">
-        <v>22.855699999999999</v>
+      <c r="PH4" t="s">
+        <v>500</v>
+      </c>
+      <c r="PI4" t="s">
+        <v>500</v>
       </c>
       <c r="PJ4">
         <v>6.4177</v>
@@ -7544,14 +7547,14 @@
       <c r="PP4">
         <v>6.6733000000000002</v>
       </c>
-      <c r="PT4">
-        <v>74.925200000000004</v>
+      <c r="PT4" t="s">
+        <v>500</v>
       </c>
       <c r="PU4" t="s">
         <v>500</v>
       </c>
-      <c r="PW4">
-        <v>16.540500000000002</v>
+      <c r="PW4" t="s">
+        <v>500</v>
       </c>
       <c r="PX4">
         <v>20.237300000000001</v>
@@ -7568,23 +7571,26 @@
       <c r="QB4">
         <v>7.7925000000000004</v>
       </c>
-      <c r="QE4">
-        <v>16.986799999999999</v>
-      </c>
-      <c r="QF4">
-        <v>10.6525</v>
-      </c>
-      <c r="QG4">
-        <v>33.804900000000004</v>
-      </c>
-      <c r="QI4">
-        <v>26.884499999999999</v>
+      <c r="QE4" t="s">
+        <v>500</v>
+      </c>
+      <c r="QF4" t="s">
+        <v>500</v>
+      </c>
+      <c r="QG4" t="s">
+        <v>500</v>
+      </c>
+      <c r="QH4" t="s">
+        <v>500</v>
+      </c>
+      <c r="QI4" t="s">
+        <v>500</v>
       </c>
       <c r="QK4">
         <v>13.685700000000001</v>
       </c>
-      <c r="QL4">
-        <v>24.765999999999998</v>
+      <c r="QL4" t="s">
+        <v>500</v>
       </c>
       <c r="QN4">
         <v>6.5580999999999996</v>
@@ -8320,23 +8326,23 @@
       <c r="GX5">
         <v>18.8781</v>
       </c>
-      <c r="GZ5">
-        <v>23.383199999999999</v>
-      </c>
-      <c r="HB5">
-        <v>13.764799999999999</v>
-      </c>
-      <c r="HC5">
-        <v>27.805199999999999</v>
-      </c>
-      <c r="HG5">
-        <v>2.6918000000000002</v>
-      </c>
-      <c r="HH5">
-        <v>6.5827</v>
-      </c>
-      <c r="HJ5">
-        <v>19.5776</v>
+      <c r="GZ5" t="s">
+        <v>500</v>
+      </c>
+      <c r="HB5" t="s">
+        <v>500</v>
+      </c>
+      <c r="HC5" t="s">
+        <v>500</v>
+      </c>
+      <c r="HG5" t="s">
+        <v>500</v>
+      </c>
+      <c r="HH5" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ5" t="s">
+        <v>500</v>
       </c>
       <c r="HL5">
         <v>16.122399999999999</v>
@@ -8368,14 +8374,14 @@
       <c r="IF5">
         <v>-80.941999999999993</v>
       </c>
-      <c r="II5">
-        <v>9.3233999999999995</v>
+      <c r="II5" t="s">
+        <v>500</v>
       </c>
       <c r="IJ5">
         <v>24.840499999999999</v>
       </c>
-      <c r="IK5">
-        <v>11.191800000000001</v>
+      <c r="IK5" t="s">
+        <v>500</v>
       </c>
       <c r="IN5">
         <v>8.2317</v>
@@ -8896,17 +8902,17 @@
       <c r="PF5">
         <v>17.115300000000001</v>
       </c>
-      <c r="PH5">
-        <v>16.694400000000002</v>
-      </c>
-      <c r="PI5">
-        <v>22.855699999999999</v>
+      <c r="PH5" t="s">
+        <v>500</v>
+      </c>
+      <c r="PI5" t="s">
+        <v>500</v>
       </c>
       <c r="PJ5">
         <v>-0.57979999999999998</v>
       </c>
-      <c r="PL5">
-        <v>20.116099999999999</v>
+      <c r="PL5" t="s">
+        <v>500</v>
       </c>
       <c r="PM5">
         <v>6.8997000000000002</v>
@@ -8920,8 +8926,8 @@
       <c r="PU5" t="s">
         <v>500</v>
       </c>
-      <c r="PW5">
-        <v>16.540500000000002</v>
+      <c r="PW5" t="s">
+        <v>500</v>
       </c>
       <c r="PX5">
         <v>22.9253</v>
@@ -8938,23 +8944,26 @@
       <c r="QB5">
         <v>10.204000000000001</v>
       </c>
-      <c r="QE5">
-        <v>16.986799999999999</v>
-      </c>
-      <c r="QF5">
-        <v>10.6525</v>
-      </c>
-      <c r="QG5">
-        <v>33.804900000000004</v>
-      </c>
-      <c r="QI5">
-        <v>26.884499999999999</v>
+      <c r="QE5" t="s">
+        <v>500</v>
+      </c>
+      <c r="QF5" t="s">
+        <v>500</v>
+      </c>
+      <c r="QG5" t="s">
+        <v>500</v>
+      </c>
+      <c r="QH5" t="s">
+        <v>500</v>
+      </c>
+      <c r="QI5" t="s">
+        <v>500</v>
       </c>
       <c r="QK5">
         <v>15.540900000000001</v>
       </c>
-      <c r="QL5">
-        <v>24.765999999999998</v>
+      <c r="QL5" t="s">
+        <v>500</v>
       </c>
       <c r="QN5">
         <v>6.8509000000000002</v>
@@ -9669,8 +9678,8 @@
       <c r="GN6">
         <v>4.6361999999999997</v>
       </c>
-      <c r="GO6">
-        <v>19.432500000000001</v>
+      <c r="GO6" t="s">
+        <v>500</v>
       </c>
       <c r="GS6">
         <v>27.7041</v>
@@ -9684,17 +9693,17 @@
       <c r="GX6">
         <v>20.057500000000001</v>
       </c>
-      <c r="GZ6">
-        <v>23.383199999999999</v>
-      </c>
-      <c r="HG6">
-        <v>2.6918000000000002</v>
-      </c>
-      <c r="HH6">
-        <v>6.5827</v>
-      </c>
-      <c r="HJ6">
-        <v>19.5776</v>
+      <c r="GZ6" t="s">
+        <v>500</v>
+      </c>
+      <c r="HG6" t="s">
+        <v>500</v>
+      </c>
+      <c r="HH6" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ6" t="s">
+        <v>500</v>
       </c>
       <c r="HL6">
         <v>16.732500000000002</v>
@@ -9726,8 +9735,8 @@
       <c r="IJ6">
         <v>29.211600000000001</v>
       </c>
-      <c r="IK6">
-        <v>11.191800000000001</v>
+      <c r="IK6" t="s">
+        <v>500</v>
       </c>
       <c r="IN6">
         <v>6.7512999999999996</v>
@@ -9999,8 +10008,8 @@
       <c r="MA6">
         <v>9.2853999999999992</v>
       </c>
-      <c r="MB6">
-        <v>-65.037999999999997</v>
+      <c r="MB6" t="s">
+        <v>500</v>
       </c>
       <c r="MC6">
         <v>9.5449000000000002</v>
@@ -10245,14 +10254,14 @@
       <c r="PF6">
         <v>18.5108</v>
       </c>
-      <c r="PH6">
-        <v>16.694400000000002</v>
-      </c>
-      <c r="PI6">
-        <v>22.855699999999999</v>
-      </c>
-      <c r="PL6">
-        <v>20.116099999999999</v>
+      <c r="PH6" t="s">
+        <v>500</v>
+      </c>
+      <c r="PI6" t="s">
+        <v>500</v>
+      </c>
+      <c r="PL6" t="s">
+        <v>500</v>
       </c>
       <c r="PM6">
         <v>4.0274000000000001</v>
@@ -10266,8 +10275,8 @@
       <c r="PU6" t="s">
         <v>500</v>
       </c>
-      <c r="PW6">
-        <v>16.540500000000002</v>
+      <c r="PW6" t="s">
+        <v>500</v>
       </c>
       <c r="PX6">
         <v>25.946400000000001</v>
@@ -10284,23 +10293,26 @@
       <c r="QB6">
         <v>12.1348</v>
       </c>
-      <c r="QE6">
-        <v>16.986799999999999</v>
-      </c>
-      <c r="QF6">
-        <v>10.6525</v>
-      </c>
-      <c r="QG6">
-        <v>33.804900000000004</v>
-      </c>
-      <c r="QI6">
-        <v>26.884499999999999</v>
+      <c r="QE6" t="s">
+        <v>500</v>
+      </c>
+      <c r="QF6" t="s">
+        <v>500</v>
+      </c>
+      <c r="QG6" t="s">
+        <v>500</v>
+      </c>
+      <c r="QH6" t="s">
+        <v>500</v>
+      </c>
+      <c r="QI6" t="s">
+        <v>500</v>
       </c>
       <c r="QK6">
         <v>17.792999999999999</v>
       </c>
-      <c r="QL6">
-        <v>24.765999999999998</v>
+      <c r="QL6" t="s">
+        <v>500</v>
       </c>
       <c r="QN6">
         <v>8.0688999999999993</v>
@@ -11003,8 +11015,8 @@
       <c r="GN7">
         <v>6.5054999999999996</v>
       </c>
-      <c r="GO7">
-        <v>19.432500000000001</v>
+      <c r="GO7" t="s">
+        <v>500</v>
       </c>
       <c r="GS7">
         <v>28.562200000000001</v>
@@ -11015,17 +11027,17 @@
       <c r="GU7">
         <v>7.2503000000000002</v>
       </c>
-      <c r="GZ7">
-        <v>23.383199999999999</v>
-      </c>
-      <c r="HG7">
-        <v>2.6918000000000002</v>
-      </c>
-      <c r="HH7">
-        <v>6.5827</v>
-      </c>
-      <c r="HJ7">
-        <v>2321999.8897000002</v>
+      <c r="GZ7" t="s">
+        <v>500</v>
+      </c>
+      <c r="HG7" t="s">
+        <v>500</v>
+      </c>
+      <c r="HH7" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ7" t="s">
+        <v>500</v>
       </c>
       <c r="HL7">
         <v>17.462</v>
@@ -11057,8 +11069,8 @@
       <c r="IJ7">
         <v>31.951699999999999</v>
       </c>
-      <c r="IK7">
-        <v>11.191800000000001</v>
+      <c r="IK7" t="s">
+        <v>500</v>
       </c>
       <c r="IN7">
         <v>7.4733999999999998</v>
@@ -11327,8 +11339,8 @@
       <c r="MA7">
         <v>9.3792000000000009</v>
       </c>
-      <c r="MB7">
-        <v>-65.037999999999997</v>
+      <c r="MB7" t="s">
+        <v>500</v>
       </c>
       <c r="MC7">
         <v>9.5361999999999991</v>
@@ -11567,14 +11579,14 @@
       <c r="PF7">
         <v>20.161899999999999</v>
       </c>
-      <c r="PH7">
-        <v>16.694400000000002</v>
-      </c>
-      <c r="PI7">
-        <v>22.855699999999999</v>
-      </c>
-      <c r="PM7">
-        <v>4.0274000000000001</v>
+      <c r="PH7" t="s">
+        <v>500</v>
+      </c>
+      <c r="PI7" t="s">
+        <v>500</v>
+      </c>
+      <c r="PM7" t="s">
+        <v>500</v>
       </c>
       <c r="PN7">
         <v>19.4328</v>
@@ -11600,23 +11612,26 @@
       <c r="QB7">
         <v>13.9246</v>
       </c>
-      <c r="QE7">
-        <v>16.986799999999999</v>
-      </c>
-      <c r="QF7">
-        <v>10.6525</v>
-      </c>
-      <c r="QG7">
-        <v>33.804900000000004</v>
-      </c>
-      <c r="QI7">
-        <v>26.884499999999999</v>
+      <c r="QE7" t="s">
+        <v>500</v>
+      </c>
+      <c r="QF7" t="s">
+        <v>500</v>
+      </c>
+      <c r="QG7" t="s">
+        <v>500</v>
+      </c>
+      <c r="QH7" t="s">
+        <v>500</v>
+      </c>
+      <c r="QI7" t="s">
+        <v>500</v>
       </c>
       <c r="QK7">
         <v>17.642099999999999</v>
       </c>
-      <c r="QL7">
-        <v>24.765999999999998</v>
+      <c r="QL7" t="s">
+        <v>500</v>
       </c>
       <c r="QN7">
         <v>8.2454000000000001</v>
@@ -12274,8 +12289,8 @@
       <c r="FV8">
         <v>6.3761000000000001</v>
       </c>
-      <c r="FW8">
-        <v>10.26</v>
+      <c r="FW8" t="s">
+        <v>500</v>
       </c>
       <c r="FY8">
         <v>21.196300000000001</v>
@@ -12283,8 +12298,8 @@
       <c r="FZ8">
         <v>-11.116400000000001</v>
       </c>
-      <c r="GA8">
-        <v>2.8645999999999998</v>
+      <c r="GA8" t="s">
+        <v>500</v>
       </c>
       <c r="GC8">
         <v>15.622</v>
@@ -12295,11 +12310,11 @@
       <c r="GE8">
         <v>9.4655000000000005</v>
       </c>
-      <c r="GF8">
-        <v>19.822199999999999</v>
-      </c>
-      <c r="GG8">
-        <v>28.242899999999999</v>
+      <c r="GF8" t="s">
+        <v>500</v>
+      </c>
+      <c r="GG8" t="s">
+        <v>500</v>
       </c>
       <c r="GJ8">
         <v>33.939900000000002</v>
@@ -12310,8 +12325,8 @@
       <c r="GN8">
         <v>7.8364000000000003</v>
       </c>
-      <c r="GO8">
-        <v>19.432500000000001</v>
+      <c r="GO8" t="s">
+        <v>500</v>
       </c>
       <c r="GS8">
         <v>25.5</v>
@@ -12319,17 +12334,20 @@
       <c r="GT8">
         <v>25.078399999999998</v>
       </c>
-      <c r="GU8">
-        <v>7.2503000000000002</v>
-      </c>
-      <c r="GZ8">
-        <v>23.383199999999999</v>
-      </c>
-      <c r="HH8">
-        <v>6.5827</v>
-      </c>
-      <c r="HJ8">
-        <v>3773999.8207</v>
+      <c r="GU8" t="s">
+        <v>500</v>
+      </c>
+      <c r="GZ8" t="s">
+        <v>500</v>
+      </c>
+      <c r="HG8" t="s">
+        <v>500</v>
+      </c>
+      <c r="HH8" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ8" t="s">
+        <v>500</v>
       </c>
       <c r="HL8">
         <v>18.685600000000001</v>
@@ -12349,8 +12367,8 @@
       <c r="HW8">
         <v>18.888300000000001</v>
       </c>
-      <c r="HX8">
-        <v>27.186</v>
+      <c r="HX8" t="s">
+        <v>500</v>
       </c>
       <c r="HZ8">
         <v>-32.099299999999999</v>
@@ -12700,8 +12718,8 @@
       <c r="MZ8">
         <v>3.036</v>
       </c>
-      <c r="NA8">
-        <v>8.7895000000000003</v>
+      <c r="NA8" t="s">
+        <v>500</v>
       </c>
       <c r="NB8">
         <v>111.6146</v>
@@ -12826,8 +12844,8 @@
       <c r="OQ8">
         <v>74.402000000000001</v>
       </c>
-      <c r="OR8">
-        <v>12.9598</v>
+      <c r="OR8" t="s">
+        <v>500</v>
       </c>
       <c r="OS8">
         <v>10.036899999999999</v>
@@ -12856,14 +12874,14 @@
       <c r="PF8">
         <v>20.668700000000001</v>
       </c>
-      <c r="PH8">
-        <v>16.694400000000002</v>
-      </c>
-      <c r="PI8">
-        <v>22.855699999999999</v>
-      </c>
-      <c r="PM8">
-        <v>4.0274000000000001</v>
+      <c r="PH8" t="s">
+        <v>500</v>
+      </c>
+      <c r="PI8" t="s">
+        <v>500</v>
+      </c>
+      <c r="PM8" t="s">
+        <v>500</v>
       </c>
       <c r="PN8">
         <v>20.632999999999999</v>
@@ -12889,20 +12907,26 @@
       <c r="QB8">
         <v>15.0762</v>
       </c>
-      <c r="QE8">
-        <v>16.986799999999999</v>
-      </c>
-      <c r="QG8">
-        <v>33.804900000000004</v>
-      </c>
-      <c r="QI8">
-        <v>26.884499999999999</v>
+      <c r="QE8" t="s">
+        <v>500</v>
+      </c>
+      <c r="QF8" t="s">
+        <v>500</v>
+      </c>
+      <c r="QG8" t="s">
+        <v>500</v>
+      </c>
+      <c r="QH8" t="s">
+        <v>500</v>
+      </c>
+      <c r="QI8" t="s">
+        <v>500</v>
       </c>
       <c r="QK8">
         <v>19.430900000000001</v>
       </c>
-      <c r="QL8">
-        <v>24.765999999999998</v>
+      <c r="QL8" t="s">
+        <v>500</v>
       </c>
       <c r="QN8">
         <v>8.3658000000000001</v>
@@ -13479,8 +13503,8 @@
       <c r="ET9">
         <v>3.8910999999999998</v>
       </c>
-      <c r="EU9">
-        <v>13.089</v>
+      <c r="EU9" t="s">
+        <v>500</v>
       </c>
       <c r="EV9">
         <v>15.234500000000001</v>
@@ -13515,8 +13539,8 @@
       <c r="FG9">
         <v>33.393300000000004</v>
       </c>
-      <c r="FH9">
-        <v>12.397</v>
+      <c r="FH9" t="s">
+        <v>500</v>
       </c>
       <c r="FI9">
         <v>1.2621</v>
@@ -13524,23 +13548,23 @@
       <c r="FJ9">
         <v>15.669600000000001</v>
       </c>
-      <c r="FK9">
-        <v>14.111599999999999</v>
-      </c>
-      <c r="FL9">
-        <v>23.807500000000001</v>
+      <c r="FK9" t="s">
+        <v>500</v>
+      </c>
+      <c r="FL9" t="s">
+        <v>500</v>
       </c>
       <c r="FM9">
         <v>14.168699999999999</v>
       </c>
-      <c r="FN9">
-        <v>22.936800000000002</v>
+      <c r="FN9" t="s">
+        <v>500</v>
       </c>
       <c r="FO9">
         <v>15.472099999999999</v>
       </c>
-      <c r="FP9">
-        <v>-2.3304</v>
+      <c r="FP9" t="s">
+        <v>500</v>
       </c>
       <c r="FQ9">
         <v>22.528300000000002</v>
@@ -13563,8 +13587,8 @@
       <c r="FZ9">
         <v>-21.457799999999999</v>
       </c>
-      <c r="GA9">
-        <v>2.8645999999999998</v>
+      <c r="GA9" t="s">
+        <v>500</v>
       </c>
       <c r="GC9">
         <v>15.4695</v>
@@ -13575,35 +13599,35 @@
       <c r="GE9">
         <v>10.172499999999999</v>
       </c>
-      <c r="GF9">
-        <v>19.822199999999999</v>
-      </c>
-      <c r="GG9">
-        <v>28.242899999999999</v>
+      <c r="GF9" t="s">
+        <v>500</v>
+      </c>
+      <c r="GG9" t="s">
+        <v>500</v>
       </c>
       <c r="GJ9">
         <v>39.5535</v>
       </c>
-      <c r="GM9">
-        <v>3.6882000000000001</v>
+      <c r="GM9" t="s">
+        <v>500</v>
       </c>
       <c r="GN9">
         <v>8.3886000000000003</v>
       </c>
-      <c r="GO9">
-        <v>19.432500000000001</v>
+      <c r="GO9" t="s">
+        <v>500</v>
       </c>
       <c r="GS9">
         <v>29.815000000000001</v>
       </c>
-      <c r="GT9">
-        <v>25.078399999999998</v>
-      </c>
-      <c r="GZ9">
-        <v>23.383199999999999</v>
-      </c>
-      <c r="HJ9">
-        <v>3773999.8207</v>
+      <c r="GT9" t="s">
+        <v>500</v>
+      </c>
+      <c r="GZ9" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ9" t="s">
+        <v>500</v>
       </c>
       <c r="HL9">
         <v>19.298400000000001</v>
@@ -13623,8 +13647,8 @@
       <c r="HZ9">
         <v>53.380800000000001</v>
       </c>
-      <c r="IF9">
-        <v>-147.3237</v>
+      <c r="IF9" t="s">
+        <v>500</v>
       </c>
       <c r="IJ9">
         <v>35.122199999999999</v>
@@ -13965,8 +13989,8 @@
       <c r="MZ9">
         <v>3.4914999999999998</v>
       </c>
-      <c r="NA9">
-        <v>8.7895000000000003</v>
+      <c r="NA9" t="s">
+        <v>500</v>
       </c>
       <c r="NB9">
         <v>24.142399999999999</v>
@@ -14022,8 +14046,8 @@
       <c r="NS9">
         <v>18.973500000000001</v>
       </c>
-      <c r="NT9">
-        <v>18.058</v>
+      <c r="NT9" t="s">
+        <v>500</v>
       </c>
       <c r="NU9">
         <v>5.9653</v>
@@ -14031,8 +14055,8 @@
       <c r="NV9">
         <v>12.6114</v>
       </c>
-      <c r="NW9">
-        <v>25.968399999999999</v>
+      <c r="NW9" t="s">
+        <v>500</v>
       </c>
       <c r="NY9">
         <v>5.5875000000000004</v>
@@ -14043,8 +14067,8 @@
       <c r="OA9">
         <v>28.338899999999999</v>
       </c>
-      <c r="OB9">
-        <v>21.725100000000001</v>
+      <c r="OB9" t="s">
+        <v>500</v>
       </c>
       <c r="OC9">
         <v>3.9582999999999999</v>
@@ -14052,8 +14076,8 @@
       <c r="OD9">
         <v>18.373699999999999</v>
       </c>
-      <c r="OE9">
-        <v>0.14649999999999999</v>
+      <c r="OE9" t="s">
+        <v>500</v>
       </c>
       <c r="OF9">
         <v>21.6907</v>
@@ -14076,14 +14100,14 @@
       <c r="ON9">
         <v>7.9722</v>
       </c>
-      <c r="OP9">
-        <v>15.424300000000001</v>
+      <c r="OP9" t="s">
+        <v>500</v>
       </c>
       <c r="OQ9">
         <v>32.964199999999998</v>
       </c>
-      <c r="OR9">
-        <v>12.9598</v>
+      <c r="OR9" t="s">
+        <v>500</v>
       </c>
       <c r="OS9">
         <v>11.2035</v>
@@ -14109,8 +14133,11 @@
       <c r="PF9">
         <v>20.040500000000002</v>
       </c>
-      <c r="PI9">
-        <v>22.855699999999999</v>
+      <c r="PH9" t="s">
+        <v>500</v>
+      </c>
+      <c r="PI9" t="s">
+        <v>500</v>
       </c>
       <c r="PN9">
         <v>21.802800000000001</v>
@@ -14136,8 +14163,8 @@
       <c r="QK9">
         <v>21.264399999999998</v>
       </c>
-      <c r="QL9">
-        <v>24.765999999999998</v>
+      <c r="QL9" t="s">
+        <v>500</v>
       </c>
       <c r="QN9">
         <v>7.7404999999999999</v>
@@ -14663,8 +14690,8 @@
       <c r="EC10">
         <v>16.803599999999999</v>
       </c>
-      <c r="ED10">
-        <v>7.8844000000000003</v>
+      <c r="ED10" t="s">
+        <v>500</v>
       </c>
       <c r="EE10">
         <v>35.145299999999999</v>
@@ -14675,8 +14702,8 @@
       <c r="EG10">
         <v>43.531799999999997</v>
       </c>
-      <c r="EH10">
-        <v>6829000</v>
+      <c r="EH10" t="s">
+        <v>500</v>
       </c>
       <c r="EI10">
         <v>12.6709</v>
@@ -14699,8 +14726,8 @@
       <c r="EP10">
         <v>19.8978</v>
       </c>
-      <c r="EQ10">
-        <v>37.698</v>
+      <c r="EQ10" t="s">
+        <v>500</v>
       </c>
       <c r="ER10">
         <v>25.916799999999999</v>
@@ -14729,8 +14756,8 @@
       <c r="FB10">
         <v>50.378700000000002</v>
       </c>
-      <c r="FC10">
-        <v>0.71360000000000001</v>
+      <c r="FC10" t="s">
+        <v>500</v>
       </c>
       <c r="FD10">
         <v>7.1013999999999999</v>
@@ -14744,8 +14771,8 @@
       <c r="FG10">
         <v>34.891599999999997</v>
       </c>
-      <c r="FH10">
-        <v>12.397</v>
+      <c r="FH10" t="s">
+        <v>500</v>
       </c>
       <c r="FI10">
         <v>1.2450000000000001</v>
@@ -14753,23 +14780,23 @@
       <c r="FJ10">
         <v>16.0304</v>
       </c>
-      <c r="FK10">
-        <v>14.111599999999999</v>
-      </c>
-      <c r="FL10">
-        <v>23.807500000000001</v>
+      <c r="FK10" t="s">
+        <v>500</v>
+      </c>
+      <c r="FL10" t="s">
+        <v>500</v>
       </c>
       <c r="FM10">
         <v>14.935600000000001</v>
       </c>
-      <c r="FN10">
-        <v>22.936800000000002</v>
+      <c r="FN10" t="s">
+        <v>500</v>
       </c>
       <c r="FO10">
         <v>16.012</v>
       </c>
-      <c r="FP10">
-        <v>-2.3304</v>
+      <c r="FP10" t="s">
+        <v>500</v>
       </c>
       <c r="FQ10">
         <v>22.277799999999999</v>
@@ -14792,8 +14819,8 @@
       <c r="FZ10">
         <v>-23.907699999999998</v>
       </c>
-      <c r="GA10">
-        <v>2.8645999999999998</v>
+      <c r="GA10" t="s">
+        <v>500</v>
       </c>
       <c r="GC10">
         <v>9.3247</v>
@@ -14804,32 +14831,32 @@
       <c r="GE10">
         <v>10.8788</v>
       </c>
-      <c r="GF10">
-        <v>19.822199999999999</v>
-      </c>
-      <c r="GG10">
-        <v>28.242899999999999</v>
+      <c r="GF10" t="s">
+        <v>500</v>
+      </c>
+      <c r="GG10" t="s">
+        <v>500</v>
       </c>
       <c r="GJ10">
         <v>37.893599999999999</v>
       </c>
-      <c r="GM10">
-        <v>3.6882000000000001</v>
+      <c r="GM10" t="s">
+        <v>500</v>
       </c>
       <c r="GN10">
         <v>8.5403000000000002</v>
       </c>
-      <c r="GO10">
-        <v>19.432500000000001</v>
-      </c>
-      <c r="GT10">
-        <v>25.078399999999998</v>
-      </c>
-      <c r="GZ10">
-        <v>23.383199999999999</v>
-      </c>
-      <c r="HJ10">
-        <v>5654999.7313999999</v>
+      <c r="GO10" t="s">
+        <v>500</v>
+      </c>
+      <c r="GT10" t="s">
+        <v>500</v>
+      </c>
+      <c r="GZ10" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ10" t="s">
+        <v>500</v>
       </c>
       <c r="HL10">
         <v>19.923200000000001</v>
@@ -14846,8 +14873,8 @@
       <c r="HW10">
         <v>17.841999999999999</v>
       </c>
-      <c r="HZ10">
-        <v>53.380800000000001</v>
+      <c r="HZ10" t="s">
+        <v>500</v>
       </c>
       <c r="IJ10">
         <v>38.811700000000002</v>
@@ -14921,8 +14948,8 @@
       <c r="JK10">
         <v>15.996700000000001</v>
       </c>
-      <c r="JL10">
-        <v>2.0935000000000001</v>
+      <c r="JL10" t="s">
+        <v>500</v>
       </c>
       <c r="JM10">
         <v>31.718299999999999</v>
@@ -14930,8 +14957,8 @@
       <c r="JN10">
         <v>24.3856</v>
       </c>
-      <c r="JO10">
-        <v>40.224699999999999</v>
+      <c r="JO10" t="s">
+        <v>500</v>
       </c>
       <c r="JP10">
         <v>19.5198</v>
@@ -14951,8 +14978,8 @@
       <c r="JU10">
         <v>7.3487</v>
       </c>
-      <c r="JV10">
-        <v>42958678.641999997</v>
+      <c r="JV10" t="s">
+        <v>500</v>
       </c>
       <c r="JW10">
         <v>4.0166000000000004</v>
@@ -15146,8 +15173,8 @@
       <c r="ML10">
         <v>3.9878999999999998</v>
       </c>
-      <c r="MM10">
-        <v>13699716.311699999</v>
+      <c r="MM10" t="s">
+        <v>500</v>
       </c>
       <c r="MN10">
         <v>13.3969</v>
@@ -15188,8 +15215,8 @@
       <c r="MZ10">
         <v>3.7059000000000002</v>
       </c>
-      <c r="NA10">
-        <v>8.7895000000000003</v>
+      <c r="NA10" t="s">
+        <v>500</v>
       </c>
       <c r="NB10">
         <v>14.0884</v>
@@ -15233,8 +15260,8 @@
       <c r="NO10">
         <v>9.9582999999999995</v>
       </c>
-      <c r="NP10">
-        <v>21.8795</v>
+      <c r="NP10" t="s">
+        <v>500</v>
       </c>
       <c r="NR10">
         <v>31.3566</v>
@@ -15242,14 +15269,14 @@
       <c r="NS10">
         <v>23.927900000000001</v>
       </c>
-      <c r="NT10">
-        <v>18.058</v>
-      </c>
-      <c r="NU10">
-        <v>5.9653</v>
-      </c>
-      <c r="NW10">
-        <v>25.968399999999999</v>
+      <c r="NT10" t="s">
+        <v>500</v>
+      </c>
+      <c r="NU10" t="s">
+        <v>500</v>
+      </c>
+      <c r="NW10" t="s">
+        <v>500</v>
       </c>
       <c r="NY10">
         <v>5.5875000000000004</v>
@@ -15260,8 +15287,8 @@
       <c r="OA10">
         <v>32.521299999999997</v>
       </c>
-      <c r="OB10">
-        <v>21.725100000000001</v>
+      <c r="OB10" t="s">
+        <v>500</v>
       </c>
       <c r="OC10">
         <v>3.2149999999999999</v>
@@ -15269,8 +15296,8 @@
       <c r="OD10">
         <v>22.290099999999999</v>
       </c>
-      <c r="OE10">
-        <v>0.14649999999999999</v>
+      <c r="OE10" t="s">
+        <v>500</v>
       </c>
       <c r="OF10">
         <v>23.328900000000001</v>
@@ -15284,20 +15311,20 @@
       <c r="OL10">
         <v>5.67</v>
       </c>
-      <c r="OM10">
-        <v>4836300</v>
+      <c r="OM10" t="s">
+        <v>500</v>
       </c>
       <c r="ON10">
         <v>7.4309000000000003</v>
       </c>
-      <c r="OP10">
-        <v>15.424300000000001</v>
+      <c r="OP10" t="s">
+        <v>500</v>
       </c>
       <c r="OQ10">
         <v>34.337800000000001</v>
       </c>
-      <c r="OR10">
-        <v>12.9598</v>
+      <c r="OR10" t="s">
+        <v>500</v>
       </c>
       <c r="OS10">
         <v>13.0098</v>
@@ -15338,8 +15365,8 @@
       <c r="QK10">
         <v>22.0975</v>
       </c>
-      <c r="QL10">
-        <v>24.765999999999998</v>
+      <c r="QL10" t="s">
+        <v>500</v>
       </c>
       <c r="QN10">
         <v>10.029199999999999</v>
@@ -15799,20 +15826,20 @@
       <c r="DJ11">
         <v>7.1226000000000003</v>
       </c>
-      <c r="DL11">
-        <v>8.9725000000000001</v>
-      </c>
-      <c r="DM11">
-        <v>4.3693</v>
+      <c r="DL11" t="s">
+        <v>500</v>
+      </c>
+      <c r="DM11" t="s">
+        <v>500</v>
       </c>
       <c r="DN11">
         <v>36.4512</v>
       </c>
-      <c r="DO11">
-        <v>12.8721</v>
-      </c>
-      <c r="DP11">
-        <v>9.2009000000000007</v>
+      <c r="DO11" t="s">
+        <v>500</v>
+      </c>
+      <c r="DP11" t="s">
+        <v>500</v>
       </c>
       <c r="DQ11">
         <v>25.254100000000001</v>
@@ -15820,8 +15847,8 @@
       <c r="DR11">
         <v>33.693399999999997</v>
       </c>
-      <c r="DS11">
-        <v>18.216200000000001</v>
+      <c r="DS11" t="s">
+        <v>500</v>
       </c>
       <c r="DT11">
         <v>11.463699999999999</v>
@@ -15844,8 +15871,8 @@
       <c r="DZ11">
         <v>16.788799999999998</v>
       </c>
-      <c r="EA11">
-        <v>9.7631999999999994</v>
+      <c r="EA11" t="s">
+        <v>500</v>
       </c>
       <c r="EB11">
         <v>37.269100000000002</v>
@@ -15853,8 +15880,8 @@
       <c r="EC11">
         <v>5.4919000000000002</v>
       </c>
-      <c r="ED11">
-        <v>7.8844000000000003</v>
+      <c r="ED11" t="s">
+        <v>500</v>
       </c>
       <c r="EE11">
         <v>34.156300000000002</v>
@@ -15865,8 +15892,8 @@
       <c r="EG11">
         <v>39.5124</v>
       </c>
-      <c r="EH11">
-        <v>2377900</v>
+      <c r="EH11" t="s">
+        <v>500</v>
       </c>
       <c r="EI11">
         <v>10.1493</v>
@@ -15889,8 +15916,8 @@
       <c r="EP11">
         <v>14.633599999999999</v>
       </c>
-      <c r="EQ11">
-        <v>37.698</v>
+      <c r="EQ11" t="s">
+        <v>500</v>
       </c>
       <c r="ER11">
         <v>29.2102</v>
@@ -15919,8 +15946,8 @@
       <c r="FB11">
         <v>48.740099999999998</v>
       </c>
-      <c r="FC11">
-        <v>0.71360000000000001</v>
+      <c r="FC11" t="s">
+        <v>500</v>
       </c>
       <c r="FD11">
         <v>4.1833999999999998</v>
@@ -15928,14 +15955,14 @@
       <c r="FE11">
         <v>9.7685999999999993</v>
       </c>
-      <c r="FF11">
-        <v>38.061300000000003</v>
+      <c r="FF11" t="s">
+        <v>500</v>
       </c>
       <c r="FG11">
         <v>35.712299999999999</v>
       </c>
-      <c r="FH11">
-        <v>12.397</v>
+      <c r="FH11" t="s">
+        <v>500</v>
       </c>
       <c r="FI11">
         <v>1.2927</v>
@@ -15943,29 +15970,29 @@
       <c r="FJ11">
         <v>11.6632</v>
       </c>
-      <c r="FK11">
-        <v>14.111599999999999</v>
-      </c>
-      <c r="FL11">
-        <v>23.807500000000001</v>
+      <c r="FK11" t="s">
+        <v>500</v>
+      </c>
+      <c r="FL11" t="s">
+        <v>500</v>
       </c>
       <c r="FM11">
         <v>15.348000000000001</v>
       </c>
-      <c r="FN11">
-        <v>22.936800000000002</v>
+      <c r="FN11" t="s">
+        <v>500</v>
       </c>
       <c r="FO11">
         <v>17.302199999999999</v>
       </c>
-      <c r="FP11">
-        <v>-2.3304</v>
+      <c r="FP11" t="s">
+        <v>500</v>
       </c>
       <c r="FQ11">
         <v>19.321999999999999</v>
       </c>
-      <c r="FR11">
-        <v>-5.2064000000000004</v>
+      <c r="FR11" t="s">
+        <v>500</v>
       </c>
       <c r="FS11">
         <v>30.324400000000001</v>
@@ -15982,8 +16009,8 @@
       <c r="FZ11">
         <v>-25.5487</v>
       </c>
-      <c r="GA11">
-        <v>2.8645999999999998</v>
+      <c r="GA11" t="s">
+        <v>500</v>
       </c>
       <c r="GC11">
         <v>7.8305999999999996</v>
@@ -15994,29 +16021,29 @@
       <c r="GE11">
         <v>14.6021</v>
       </c>
-      <c r="GF11">
-        <v>19.822199999999999</v>
-      </c>
-      <c r="GG11">
-        <v>28.242899999999999</v>
+      <c r="GF11" t="s">
+        <v>500</v>
+      </c>
+      <c r="GG11" t="s">
+        <v>500</v>
       </c>
       <c r="GJ11">
         <v>38.185499999999998</v>
       </c>
-      <c r="GM11">
-        <v>3.6882000000000001</v>
+      <c r="GM11" t="s">
+        <v>500</v>
       </c>
       <c r="GN11">
         <v>9.3704000000000001</v>
       </c>
-      <c r="GO11">
-        <v>19.432500000000001</v>
-      </c>
-      <c r="GT11">
-        <v>25.078399999999998</v>
-      </c>
-      <c r="HJ11">
-        <v>5561999.7357999999</v>
+      <c r="GO11" t="s">
+        <v>500</v>
+      </c>
+      <c r="GT11" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ11" t="s">
+        <v>500</v>
       </c>
       <c r="HL11">
         <v>14.9656</v>
@@ -16033,8 +16060,8 @@
       <c r="HW11">
         <v>20.157</v>
       </c>
-      <c r="HZ11">
-        <v>53.380800000000001</v>
+      <c r="HZ11" t="s">
+        <v>500</v>
       </c>
       <c r="IJ11">
         <v>23.584</v>
@@ -16108,14 +16135,14 @@
       <c r="JK11">
         <v>5.2948000000000004</v>
       </c>
-      <c r="JL11">
-        <v>2.0935000000000001</v>
+      <c r="JL11" t="s">
+        <v>500</v>
       </c>
       <c r="JM11">
         <v>19.463200000000001</v>
       </c>
-      <c r="JO11">
-        <v>40.224699999999999</v>
+      <c r="JO11" t="s">
+        <v>500</v>
       </c>
       <c r="JP11">
         <v>-92.142200000000003</v>
@@ -16132,8 +16159,8 @@
       <c r="JU11">
         <v>7.2953000000000001</v>
       </c>
-      <c r="JV11">
-        <v>42958678.641999997</v>
+      <c r="JV11" t="s">
+        <v>500</v>
       </c>
       <c r="JW11">
         <v>-2.2031999999999998</v>
@@ -16318,8 +16345,8 @@
       <c r="MI11">
         <v>11.385199999999999</v>
       </c>
-      <c r="MJ11">
-        <v>1.3425</v>
+      <c r="MJ11" t="s">
+        <v>500</v>
       </c>
       <c r="MK11">
         <v>17.284700000000001</v>
@@ -16327,8 +16354,8 @@
       <c r="ML11">
         <v>3.1713</v>
       </c>
-      <c r="MM11">
-        <v>15729196.050799999</v>
+      <c r="MM11" t="s">
+        <v>500</v>
       </c>
       <c r="MN11">
         <v>13.388400000000001</v>
@@ -16369,8 +16396,8 @@
       <c r="MZ11">
         <v>4.01</v>
       </c>
-      <c r="NA11">
-        <v>8.7895000000000003</v>
+      <c r="NA11" t="s">
+        <v>500</v>
       </c>
       <c r="NB11">
         <v>0.91369999999999996</v>
@@ -16411,8 +16438,8 @@
       <c r="NO11">
         <v>10.420500000000001</v>
       </c>
-      <c r="NP11">
-        <v>21.8795</v>
+      <c r="NP11" t="s">
+        <v>500</v>
       </c>
       <c r="NR11">
         <v>23.575199999999999</v>
@@ -16420,14 +16447,14 @@
       <c r="NS11">
         <v>18.716200000000001</v>
       </c>
-      <c r="NT11">
-        <v>18.058</v>
-      </c>
-      <c r="NU11">
-        <v>5.9653</v>
-      </c>
-      <c r="NW11">
-        <v>25.968399999999999</v>
+      <c r="NT11" t="s">
+        <v>500</v>
+      </c>
+      <c r="NU11" t="s">
+        <v>500</v>
+      </c>
+      <c r="NW11" t="s">
+        <v>500</v>
       </c>
       <c r="NY11">
         <v>5.0909000000000004</v>
@@ -16438,8 +16465,8 @@
       <c r="OA11">
         <v>24.168299999999999</v>
       </c>
-      <c r="OB11">
-        <v>21.725100000000001</v>
+      <c r="OB11" t="s">
+        <v>500</v>
       </c>
       <c r="OC11">
         <v>3.5095999999999998</v>
@@ -16447,8 +16474,8 @@
       <c r="OD11">
         <v>20.6556</v>
       </c>
-      <c r="OE11">
-        <v>0.14649999999999999</v>
+      <c r="OE11" t="s">
+        <v>500</v>
       </c>
       <c r="OF11">
         <v>23.164999999999999</v>
@@ -16462,20 +16489,20 @@
       <c r="OL11">
         <v>5.8467000000000002</v>
       </c>
-      <c r="OM11">
-        <v>3840300</v>
+      <c r="OM11" t="s">
+        <v>500</v>
       </c>
       <c r="ON11">
         <v>4.5465</v>
       </c>
-      <c r="OP11">
-        <v>15.424300000000001</v>
+      <c r="OP11" t="s">
+        <v>500</v>
       </c>
       <c r="OQ11">
         <v>28.269300000000001</v>
       </c>
-      <c r="OR11">
-        <v>12.9598</v>
+      <c r="OR11" t="s">
+        <v>500</v>
       </c>
       <c r="OS11">
         <v>14.542299999999999</v>
@@ -16510,8 +16537,8 @@
       <c r="QK11">
         <v>22.852399999999999</v>
       </c>
-      <c r="QL11">
-        <v>24.765999999999998</v>
+      <c r="QL11" t="s">
+        <v>500</v>
       </c>
       <c r="QN11">
         <v>11.1838</v>
@@ -16953,11 +16980,11 @@
       <c r="DB12">
         <v>25.713899999999999</v>
       </c>
-      <c r="DC12">
-        <v>4.9379</v>
-      </c>
-      <c r="DE12">
-        <v>15.2432</v>
+      <c r="DC12" t="s">
+        <v>500</v>
+      </c>
+      <c r="DE12" t="s">
+        <v>500</v>
       </c>
       <c r="DF12">
         <v>6.05</v>
@@ -16965,20 +16992,20 @@
       <c r="DH12">
         <v>21.798400000000001</v>
       </c>
-      <c r="DJ12">
-        <v>7.1226000000000003</v>
-      </c>
-      <c r="DL12">
-        <v>8.9725000000000001</v>
-      </c>
-      <c r="DM12">
-        <v>4.3693</v>
+      <c r="DJ12" t="s">
+        <v>500</v>
+      </c>
+      <c r="DL12" t="s">
+        <v>500</v>
+      </c>
+      <c r="DM12" t="s">
+        <v>500</v>
       </c>
       <c r="DN12">
         <v>41.343899999999998</v>
       </c>
-      <c r="DP12">
-        <v>9.2009000000000007</v>
+      <c r="DP12" t="s">
+        <v>500</v>
       </c>
       <c r="DQ12">
         <v>23.4727</v>
@@ -16986,8 +17013,8 @@
       <c r="DR12">
         <v>35.817500000000003</v>
       </c>
-      <c r="DS12">
-        <v>18.216200000000001</v>
+      <c r="DS12" t="s">
+        <v>500</v>
       </c>
       <c r="DT12">
         <v>13.601800000000001</v>
@@ -17010,8 +17037,8 @@
       <c r="DZ12">
         <v>19.151499999999999</v>
       </c>
-      <c r="EA12">
-        <v>9.7631999999999994</v>
+      <c r="EA12" t="s">
+        <v>500</v>
       </c>
       <c r="EB12">
         <v>41.731000000000002</v>
@@ -17019,8 +17046,8 @@
       <c r="EC12">
         <v>8.3911999999999995</v>
       </c>
-      <c r="ED12">
-        <v>7.8844000000000003</v>
+      <c r="ED12" t="s">
+        <v>500</v>
       </c>
       <c r="EE12">
         <v>32.692100000000003</v>
@@ -17031,8 +17058,8 @@
       <c r="EG12">
         <v>47.549799999999998</v>
       </c>
-      <c r="EH12">
-        <v>2377900</v>
+      <c r="EH12" t="s">
+        <v>500</v>
       </c>
       <c r="EI12">
         <v>11.3269</v>
@@ -17055,8 +17082,8 @@
       <c r="EP12">
         <v>11.229100000000001</v>
       </c>
-      <c r="EQ12">
-        <v>37.698</v>
+      <c r="EQ12" t="s">
+        <v>500</v>
       </c>
       <c r="ER12">
         <v>30.204599999999999</v>
@@ -17085,8 +17112,8 @@
       <c r="FB12">
         <v>35.287500000000001</v>
       </c>
-      <c r="FC12">
-        <v>0.71360000000000001</v>
+      <c r="FC12" t="s">
+        <v>500</v>
       </c>
       <c r="FD12">
         <v>3.7995999999999999</v>
@@ -17094,8 +17121,8 @@
       <c r="FE12">
         <v>10.378299999999999</v>
       </c>
-      <c r="FF12">
-        <v>38.061300000000003</v>
+      <c r="FF12" t="s">
+        <v>500</v>
       </c>
       <c r="FG12">
         <v>37.6997</v>
@@ -17106,29 +17133,29 @@
       <c r="FJ12">
         <v>18.235199999999999</v>
       </c>
-      <c r="FK12">
-        <v>14.111599999999999</v>
-      </c>
-      <c r="FL12">
-        <v>23.807500000000001</v>
+      <c r="FK12" t="s">
+        <v>500</v>
+      </c>
+      <c r="FL12" t="s">
+        <v>500</v>
       </c>
       <c r="FM12">
         <v>16.633299999999998</v>
       </c>
-      <c r="FN12">
-        <v>22.936800000000002</v>
+      <c r="FN12" t="s">
+        <v>500</v>
       </c>
       <c r="FO12">
         <v>20.5806</v>
       </c>
-      <c r="FP12">
-        <v>-2.3304</v>
+      <c r="FP12" t="s">
+        <v>500</v>
       </c>
       <c r="FQ12">
         <v>25.6174</v>
       </c>
-      <c r="FR12">
-        <v>-5.2064000000000004</v>
+      <c r="FR12" t="s">
+        <v>500</v>
       </c>
       <c r="FS12">
         <v>30.946300000000001</v>
@@ -17142,8 +17169,8 @@
       <c r="FY12">
         <v>32.064</v>
       </c>
-      <c r="GA12">
-        <v>2.8645999999999998</v>
+      <c r="GA12" t="s">
+        <v>500</v>
       </c>
       <c r="GC12">
         <v>8.6049000000000007</v>
@@ -17154,29 +17181,29 @@
       <c r="GE12">
         <v>14.488899999999999</v>
       </c>
-      <c r="GF12">
-        <v>19.822199999999999</v>
-      </c>
-      <c r="GG12">
-        <v>28.242899999999999</v>
+      <c r="GF12" t="s">
+        <v>500</v>
+      </c>
+      <c r="GG12" t="s">
+        <v>500</v>
       </c>
       <c r="GJ12">
         <v>47.380299999999998</v>
       </c>
-      <c r="GM12">
-        <v>3.6882000000000001</v>
+      <c r="GM12" t="s">
+        <v>500</v>
       </c>
       <c r="GN12">
         <v>10.2409</v>
       </c>
-      <c r="GO12">
-        <v>19.432500000000001</v>
-      </c>
-      <c r="GT12">
-        <v>25.078399999999998</v>
-      </c>
-      <c r="HJ12">
-        <v>2716499.8709999998</v>
+      <c r="GO12" t="s">
+        <v>500</v>
+      </c>
+      <c r="GT12" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ12" t="s">
+        <v>500</v>
       </c>
       <c r="HL12">
         <v>9.0401000000000007</v>
@@ -17193,8 +17220,8 @@
       <c r="HW12">
         <v>24.4984</v>
       </c>
-      <c r="HZ12">
-        <v>53.380800000000001</v>
+      <c r="HZ12" t="s">
+        <v>500</v>
       </c>
       <c r="IJ12">
         <v>31.0838</v>
@@ -17268,14 +17295,14 @@
       <c r="JK12">
         <v>2.2806999999999999</v>
       </c>
-      <c r="JL12">
-        <v>2.0935000000000001</v>
+      <c r="JL12" t="s">
+        <v>500</v>
       </c>
       <c r="JM12">
         <v>10.4122</v>
       </c>
-      <c r="JO12">
-        <v>40.224699999999999</v>
+      <c r="JO12" t="s">
+        <v>500</v>
       </c>
       <c r="JP12">
         <v>-94.9011</v>
@@ -17292,8 +17319,8 @@
       <c r="JU12">
         <v>8.2513000000000005</v>
       </c>
-      <c r="JV12">
-        <v>42958678.641999997</v>
+      <c r="JV12" t="s">
+        <v>500</v>
       </c>
       <c r="JW12">
         <v>-0.97309999999999997</v>
@@ -17478,8 +17505,8 @@
       <c r="MI12">
         <v>14.8996</v>
       </c>
-      <c r="MJ12">
-        <v>1.3425</v>
+      <c r="MJ12" t="s">
+        <v>500</v>
       </c>
       <c r="MK12">
         <v>18.672799999999999</v>
@@ -17487,8 +17514,8 @@
       <c r="ML12">
         <v>6.5448000000000004</v>
       </c>
-      <c r="MM12">
-        <v>19117977.528099999</v>
+      <c r="MM12" t="s">
+        <v>500</v>
       </c>
       <c r="MN12">
         <v>13.92</v>
@@ -17550,8 +17577,8 @@
       <c r="NH12">
         <v>29.5943</v>
       </c>
-      <c r="NI12">
-        <v>7.3757000000000001</v>
+      <c r="NI12" t="s">
+        <v>500</v>
       </c>
       <c r="NJ12">
         <v>11.7912</v>
@@ -17568,8 +17595,8 @@
       <c r="NO12">
         <v>11.4619</v>
       </c>
-      <c r="NP12">
-        <v>21.8795</v>
+      <c r="NP12" t="s">
+        <v>500</v>
       </c>
       <c r="NR12">
         <v>27.0871</v>
@@ -17577,11 +17604,11 @@
       <c r="NS12">
         <v>20.245799999999999</v>
       </c>
-      <c r="NT12">
-        <v>18.058</v>
-      </c>
-      <c r="NU12">
-        <v>5.9653</v>
+      <c r="NT12" t="s">
+        <v>500</v>
+      </c>
+      <c r="NU12" t="s">
+        <v>500</v>
       </c>
       <c r="NZ12">
         <v>27.324000000000002</v>
@@ -17589,8 +17616,8 @@
       <c r="OA12">
         <v>26.712900000000001</v>
       </c>
-      <c r="OB12">
-        <v>21.725100000000001</v>
+      <c r="OB12" t="s">
+        <v>500</v>
       </c>
       <c r="OC12">
         <v>4.3653000000000004</v>
@@ -17598,8 +17625,8 @@
       <c r="OD12">
         <v>22.339600000000001</v>
       </c>
-      <c r="OE12">
-        <v>0.14649999999999999</v>
+      <c r="OE12" t="s">
+        <v>500</v>
       </c>
       <c r="OF12">
         <v>23.473700000000001</v>
@@ -17613,17 +17640,17 @@
       <c r="OL12">
         <v>6.5049000000000001</v>
       </c>
-      <c r="OM12">
-        <v>3733500</v>
-      </c>
-      <c r="ON12">
-        <v>4.5465</v>
+      <c r="OM12" t="s">
+        <v>500</v>
+      </c>
+      <c r="ON12" t="s">
+        <v>500</v>
       </c>
       <c r="OQ12">
         <v>30.195499999999999</v>
       </c>
-      <c r="OR12">
-        <v>12.9598</v>
+      <c r="OR12" t="s">
+        <v>500</v>
       </c>
       <c r="OS12">
         <v>15.341900000000001</v>
@@ -18068,26 +18095,26 @@
       <c r="CS13">
         <v>40.561399999999999</v>
       </c>
-      <c r="CT13">
-        <v>26.990300000000001</v>
+      <c r="CT13" t="s">
+        <v>500</v>
       </c>
       <c r="CU13">
         <v>44.506500000000003</v>
       </c>
-      <c r="CV13">
-        <v>21.073799999999999</v>
+      <c r="CV13" t="s">
+        <v>500</v>
       </c>
       <c r="CW13">
         <v>34.362299999999998</v>
       </c>
-      <c r="CX13">
-        <v>0.39319999999999999</v>
+      <c r="CX13" t="s">
+        <v>500</v>
       </c>
       <c r="CY13">
         <v>3.9702000000000002</v>
       </c>
-      <c r="CZ13">
-        <v>37.5595</v>
+      <c r="CZ13" t="s">
+        <v>500</v>
       </c>
       <c r="DA13">
         <v>7.1786000000000003</v>
@@ -18095,8 +18122,8 @@
       <c r="DB13">
         <v>27.659600000000001</v>
       </c>
-      <c r="DE13">
-        <v>15.2432</v>
+      <c r="DE13" t="s">
+        <v>500</v>
       </c>
       <c r="DF13">
         <v>6.5472999999999999</v>
@@ -18104,20 +18131,20 @@
       <c r="DH13">
         <v>27.068999999999999</v>
       </c>
-      <c r="DJ13">
-        <v>7.1226000000000003</v>
-      </c>
-      <c r="DL13">
-        <v>8.9725000000000001</v>
-      </c>
-      <c r="DM13">
-        <v>4.3693</v>
+      <c r="DJ13" t="s">
+        <v>500</v>
+      </c>
+      <c r="DL13" t="s">
+        <v>500</v>
+      </c>
+      <c r="DM13" t="s">
+        <v>500</v>
       </c>
       <c r="DN13">
         <v>46.178699999999999</v>
       </c>
-      <c r="DP13">
-        <v>9.2009000000000007</v>
+      <c r="DP13" t="s">
+        <v>500</v>
       </c>
       <c r="DQ13">
         <v>22.546800000000001</v>
@@ -18125,8 +18152,8 @@
       <c r="DR13">
         <v>39.965800000000002</v>
       </c>
-      <c r="DS13">
-        <v>18.216200000000001</v>
+      <c r="DS13" t="s">
+        <v>500</v>
       </c>
       <c r="DT13">
         <v>12.5412</v>
@@ -18140,8 +18167,8 @@
       <c r="DW13">
         <v>16.984200000000001</v>
       </c>
-      <c r="DX13">
-        <v>-22.691099999999999</v>
+      <c r="DX13" t="s">
+        <v>500</v>
       </c>
       <c r="DY13">
         <v>13.137499999999999</v>
@@ -18149,8 +18176,8 @@
       <c r="DZ13">
         <v>20.4834</v>
       </c>
-      <c r="EA13">
-        <v>9.7631999999999994</v>
+      <c r="EA13" t="s">
+        <v>500</v>
       </c>
       <c r="EB13">
         <v>47.919800000000002</v>
@@ -18158,8 +18185,8 @@
       <c r="EC13">
         <v>5.5890000000000004</v>
       </c>
-      <c r="ED13">
-        <v>7.8844000000000003</v>
+      <c r="ED13" t="s">
+        <v>500</v>
       </c>
       <c r="EE13">
         <v>33.863599999999998</v>
@@ -18170,8 +18197,8 @@
       <c r="EG13">
         <v>56.264299999999999</v>
       </c>
-      <c r="EH13">
-        <v>2377900</v>
+      <c r="EH13" t="s">
+        <v>500</v>
       </c>
       <c r="EI13">
         <v>11.341699999999999</v>
@@ -18194,8 +18221,8 @@
       <c r="EP13">
         <v>15.874599999999999</v>
       </c>
-      <c r="EQ13">
-        <v>37.698</v>
+      <c r="EQ13" t="s">
+        <v>500</v>
       </c>
       <c r="ER13">
         <v>32.481999999999999</v>
@@ -18221,8 +18248,8 @@
       <c r="FB13">
         <v>36.344299999999997</v>
       </c>
-      <c r="FC13">
-        <v>0.71360000000000001</v>
+      <c r="FC13" t="s">
+        <v>500</v>
       </c>
       <c r="FD13">
         <v>6.1646999999999998</v>
@@ -18230,8 +18257,8 @@
       <c r="FE13">
         <v>10.7798</v>
       </c>
-      <c r="FF13">
-        <v>38.061300000000003</v>
+      <c r="FF13" t="s">
+        <v>500</v>
       </c>
       <c r="FG13">
         <v>39.249299999999998</v>
@@ -18242,26 +18269,26 @@
       <c r="FJ13">
         <v>22.525600000000001</v>
       </c>
-      <c r="FK13">
-        <v>14.111599999999999</v>
+      <c r="FK13" t="s">
+        <v>500</v>
       </c>
       <c r="FM13">
         <v>18.067799999999998</v>
       </c>
-      <c r="FN13">
-        <v>22.936800000000002</v>
+      <c r="FN13" t="s">
+        <v>500</v>
       </c>
       <c r="FO13">
         <v>23.779900000000001</v>
       </c>
-      <c r="FP13">
-        <v>-2.3304</v>
+      <c r="FP13" t="s">
+        <v>500</v>
       </c>
       <c r="FQ13">
         <v>28.253799999999998</v>
       </c>
-      <c r="FR13">
-        <v>-5.2064000000000004</v>
+      <c r="FR13" t="s">
+        <v>500</v>
       </c>
       <c r="FS13">
         <v>33.4803</v>
@@ -18275,8 +18302,8 @@
       <c r="FY13">
         <v>30.767700000000001</v>
       </c>
-      <c r="GA13">
-        <v>2.8645999999999998</v>
+      <c r="GA13" t="s">
+        <v>500</v>
       </c>
       <c r="GC13">
         <v>7.9470999999999998</v>
@@ -18287,23 +18314,23 @@
       <c r="GE13">
         <v>12.4581</v>
       </c>
-      <c r="GF13">
-        <v>19.822199999999999</v>
+      <c r="GF13" t="s">
+        <v>500</v>
       </c>
       <c r="GJ13">
         <v>41.429600000000001</v>
       </c>
-      <c r="GM13">
-        <v>3.6882000000000001</v>
+      <c r="GM13" t="s">
+        <v>500</v>
       </c>
       <c r="GN13">
         <v>13.287000000000001</v>
       </c>
-      <c r="GO13">
-        <v>19.432500000000001</v>
-      </c>
-      <c r="HJ13">
-        <v>2716499.8709999998</v>
+      <c r="GO13" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ13" t="s">
+        <v>500</v>
       </c>
       <c r="HL13">
         <v>9.5161999999999995</v>
@@ -18374,8 +18401,8 @@
       <c r="JE13">
         <v>3.4249000000000001</v>
       </c>
-      <c r="JF13">
-        <v>7.4432999999999998</v>
+      <c r="JF13" t="s">
+        <v>500</v>
       </c>
       <c r="JG13">
         <v>5.7434000000000003</v>
@@ -18392,14 +18419,14 @@
       <c r="JK13">
         <v>-0.25559999999999999</v>
       </c>
-      <c r="JL13">
-        <v>2.0935000000000001</v>
+      <c r="JL13" t="s">
+        <v>500</v>
       </c>
       <c r="JM13">
         <v>8.3265999999999991</v>
       </c>
-      <c r="JO13">
-        <v>40.224699999999999</v>
+      <c r="JO13" t="s">
+        <v>500</v>
       </c>
       <c r="JP13">
         <v>-121.2453</v>
@@ -18599,8 +18626,8 @@
       <c r="MI13">
         <v>16.746600000000001</v>
       </c>
-      <c r="MJ13">
-        <v>1.3425</v>
+      <c r="MJ13" t="s">
+        <v>500</v>
       </c>
       <c r="MK13">
         <v>20.648900000000001</v>
@@ -18608,8 +18635,8 @@
       <c r="ML13">
         <v>7.8037999999999998</v>
       </c>
-      <c r="MM13">
-        <v>21303370.786499999</v>
+      <c r="MM13" t="s">
+        <v>500</v>
       </c>
       <c r="MN13">
         <v>16.639099999999999</v>
@@ -18671,8 +18698,8 @@
       <c r="NH13">
         <v>32.366900000000001</v>
       </c>
-      <c r="NI13">
-        <v>7.3757000000000001</v>
+      <c r="NI13" t="s">
+        <v>500</v>
       </c>
       <c r="NJ13">
         <v>10.495699999999999</v>
@@ -18689,8 +18716,8 @@
       <c r="NO13">
         <v>10.84</v>
       </c>
-      <c r="NP13">
-        <v>21.8795</v>
+      <c r="NP13" t="s">
+        <v>500</v>
       </c>
       <c r="NR13">
         <v>34.714300000000001</v>
@@ -18698,8 +18725,8 @@
       <c r="NS13">
         <v>23.038</v>
       </c>
-      <c r="NU13">
-        <v>5.9653</v>
+      <c r="NU13" t="s">
+        <v>500</v>
       </c>
       <c r="NZ13">
         <v>29.710899999999999</v>
@@ -18725,17 +18752,17 @@
       <c r="OL13">
         <v>7.9537000000000004</v>
       </c>
-      <c r="OM13">
-        <v>3175100</v>
-      </c>
-      <c r="ON13">
-        <v>4.5465</v>
+      <c r="OM13" t="s">
+        <v>500</v>
+      </c>
+      <c r="ON13" t="s">
+        <v>500</v>
       </c>
       <c r="OQ13">
         <v>31.887499999999999</v>
       </c>
-      <c r="OR13">
-        <v>12.9598</v>
+      <c r="OR13" t="s">
+        <v>500</v>
       </c>
       <c r="OS13">
         <v>16.6953</v>
@@ -19168,14 +19195,14 @@
       <c r="CS14">
         <v>48.620199999999997</v>
       </c>
-      <c r="CT14">
-        <v>26.990300000000001</v>
+      <c r="CT14" t="s">
+        <v>500</v>
       </c>
       <c r="CU14">
         <v>47.38</v>
       </c>
-      <c r="CV14">
-        <v>21.073799999999999</v>
+      <c r="CV14" t="s">
+        <v>500</v>
       </c>
       <c r="CW14">
         <v>35.5212</v>
@@ -19183,8 +19210,8 @@
       <c r="CY14">
         <v>1.5147999999999999</v>
       </c>
-      <c r="CZ14">
-        <v>37.5595</v>
+      <c r="CZ14" t="s">
+        <v>500</v>
       </c>
       <c r="DA14">
         <v>5.4638</v>
@@ -19192,8 +19219,8 @@
       <c r="DB14">
         <v>29.315100000000001</v>
       </c>
-      <c r="DE14">
-        <v>15.2432</v>
+      <c r="DE14" t="s">
+        <v>500</v>
       </c>
       <c r="DF14">
         <v>6.4138000000000002</v>
@@ -19201,17 +19228,17 @@
       <c r="DH14">
         <v>26.0671</v>
       </c>
-      <c r="DJ14">
-        <v>7.1226000000000003</v>
-      </c>
-      <c r="DM14">
-        <v>4.3693</v>
+      <c r="DJ14" t="s">
+        <v>500</v>
+      </c>
+      <c r="DM14" t="s">
+        <v>500</v>
       </c>
       <c r="DN14">
         <v>40.710599999999999</v>
       </c>
-      <c r="DP14">
-        <v>9.2009000000000007</v>
+      <c r="DP14" t="s">
+        <v>500</v>
       </c>
       <c r="DQ14">
         <v>23.598800000000001</v>
@@ -19219,8 +19246,8 @@
       <c r="DR14">
         <v>46.386699999999998</v>
       </c>
-      <c r="DS14">
-        <v>18.216200000000001</v>
+      <c r="DS14" t="s">
+        <v>500</v>
       </c>
       <c r="DT14">
         <v>12.817500000000001</v>
@@ -19240,8 +19267,8 @@
       <c r="DZ14">
         <v>21.693200000000001</v>
       </c>
-      <c r="EA14">
-        <v>9.7631999999999994</v>
+      <c r="EA14" t="s">
+        <v>500</v>
       </c>
       <c r="EB14">
         <v>50.743200000000002</v>
@@ -19258,8 +19285,8 @@
       <c r="EG14">
         <v>61.510399999999997</v>
       </c>
-      <c r="EH14">
-        <v>2377900</v>
+      <c r="EH14" t="s">
+        <v>500</v>
       </c>
       <c r="EI14">
         <v>10.6953</v>
@@ -19312,8 +19339,8 @@
       <c r="FE14">
         <v>9.8422000000000001</v>
       </c>
-      <c r="FF14">
-        <v>38.061300000000003</v>
+      <c r="FF14" t="s">
+        <v>500</v>
       </c>
       <c r="FG14">
         <v>40.492199999999997</v>
@@ -19324,8 +19351,8 @@
       <c r="FJ14">
         <v>25.582599999999999</v>
       </c>
-      <c r="FK14">
-        <v>14.111599999999999</v>
+      <c r="FK14" t="s">
+        <v>500</v>
       </c>
       <c r="FM14">
         <v>19.354900000000001</v>
@@ -19333,14 +19360,14 @@
       <c r="FO14">
         <v>27.23</v>
       </c>
-      <c r="FP14">
-        <v>-2.3304</v>
+      <c r="FP14" t="s">
+        <v>500</v>
       </c>
       <c r="FQ14">
         <v>27.91</v>
       </c>
-      <c r="FR14">
-        <v>-5.2064000000000004</v>
+      <c r="FR14" t="s">
+        <v>500</v>
       </c>
       <c r="FS14">
         <v>24.363600000000002</v>
@@ -19369,11 +19396,11 @@
       <c r="GN14">
         <v>14.001200000000001</v>
       </c>
-      <c r="GO14">
-        <v>78691176.470599994</v>
-      </c>
-      <c r="HJ14">
-        <v>4433000</v>
+      <c r="GO14" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ14" t="s">
+        <v>500</v>
       </c>
       <c r="HL14">
         <v>10.088100000000001</v>
@@ -19432,8 +19459,8 @@
       <c r="JA14">
         <v>17.435400000000001</v>
       </c>
-      <c r="JB14">
-        <v>3.3784999999999998</v>
+      <c r="JB14" t="s">
+        <v>500</v>
       </c>
       <c r="JC14">
         <v>7.5846999999999998</v>
@@ -19441,8 +19468,8 @@
       <c r="JE14">
         <v>4.4569000000000001</v>
       </c>
-      <c r="JF14">
-        <v>7.4432999999999998</v>
+      <c r="JF14" t="s">
+        <v>500</v>
       </c>
       <c r="JG14">
         <v>4.8795000000000002</v>
@@ -19459,8 +19486,8 @@
       <c r="JK14">
         <v>-1.0807</v>
       </c>
-      <c r="JL14">
-        <v>2.0935000000000001</v>
+      <c r="JL14" t="s">
+        <v>500</v>
       </c>
       <c r="JM14">
         <v>5.9492000000000003</v>
@@ -19657,14 +19684,17 @@
       <c r="MI14">
         <v>17.6431</v>
       </c>
+      <c r="MJ14" t="s">
+        <v>500</v>
+      </c>
       <c r="MK14">
         <v>20.0807</v>
       </c>
       <c r="ML14">
         <v>6.3971</v>
       </c>
-      <c r="MM14">
-        <v>23787921.348299999</v>
+      <c r="MM14" t="s">
+        <v>500</v>
       </c>
       <c r="MN14">
         <v>16.280200000000001</v>
@@ -19771,11 +19801,11 @@
       <c r="OL14">
         <v>7.9957000000000003</v>
       </c>
-      <c r="OM14">
-        <v>2682100</v>
-      </c>
-      <c r="ON14">
-        <v>4.5465</v>
+      <c r="OM14" t="s">
+        <v>500</v>
+      </c>
+      <c r="ON14" t="s">
+        <v>500</v>
       </c>
       <c r="OQ14">
         <v>11.2285</v>
@@ -20199,14 +20229,14 @@
       <c r="CS15">
         <v>55.168999999999997</v>
       </c>
-      <c r="CT15">
-        <v>26.990300000000001</v>
+      <c r="CT15" t="s">
+        <v>500</v>
       </c>
       <c r="CU15">
         <v>49.664999999999999</v>
       </c>
-      <c r="CV15">
-        <v>21.073799999999999</v>
+      <c r="CV15" t="s">
+        <v>500</v>
       </c>
       <c r="CW15">
         <v>37.657299999999999</v>
@@ -20214,8 +20244,8 @@
       <c r="CY15">
         <v>0.92259999999999998</v>
       </c>
-      <c r="CZ15">
-        <v>37.5595</v>
+      <c r="CZ15" t="s">
+        <v>500</v>
       </c>
       <c r="DA15">
         <v>2.7490999999999999</v>
@@ -20229,8 +20259,8 @@
       <c r="DH15">
         <v>27.727699999999999</v>
       </c>
-      <c r="DJ15">
-        <v>7.1226000000000003</v>
+      <c r="DJ15" t="s">
+        <v>500</v>
       </c>
       <c r="DN15">
         <v>39.772599999999997</v>
@@ -20274,8 +20304,8 @@
       <c r="EG15">
         <v>67.070099999999996</v>
       </c>
-      <c r="EH15">
-        <v>2377900</v>
+      <c r="EH15" t="s">
+        <v>500</v>
       </c>
       <c r="EI15">
         <v>13.2288</v>
@@ -20370,11 +20400,11 @@
       <c r="GN15">
         <v>13.8475</v>
       </c>
-      <c r="GO15">
-        <v>66617647.058799997</v>
-      </c>
-      <c r="HJ15">
-        <v>3322000</v>
+      <c r="GO15" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ15" t="s">
+        <v>500</v>
       </c>
       <c r="HL15">
         <v>10.780200000000001</v>
@@ -20454,8 +20484,8 @@
       <c r="JK15">
         <v>-1.0887</v>
       </c>
-      <c r="JL15">
-        <v>2.0935000000000001</v>
+      <c r="JL15" t="s">
+        <v>500</v>
       </c>
       <c r="JM15">
         <v>0.9748</v>
@@ -20511,8 +20541,8 @@
       <c r="KJ15">
         <v>8.5536999999999992</v>
       </c>
-      <c r="KL15">
-        <v>30.9651</v>
+      <c r="KL15" t="s">
+        <v>500</v>
       </c>
       <c r="KM15">
         <v>5.0254000000000003</v>
@@ -20655,8 +20685,8 @@
       <c r="ML15">
         <v>6.9184999999999999</v>
       </c>
-      <c r="MM15">
-        <v>22820476.8583</v>
+      <c r="MM15" t="s">
+        <v>500</v>
       </c>
       <c r="MN15">
         <v>16.8627</v>
@@ -20763,8 +20793,8 @@
       <c r="OL15">
         <v>8.8581000000000003</v>
       </c>
-      <c r="OM15">
-        <v>1968600</v>
+      <c r="OM15" t="s">
+        <v>500</v>
       </c>
       <c r="OQ15">
         <v>11.5182</v>
@@ -21185,8 +21215,8 @@
       <c r="CY16">
         <v>1.5993999999999999</v>
       </c>
-      <c r="CZ16">
-        <v>37.5595</v>
+      <c r="CZ16" t="s">
+        <v>500</v>
       </c>
       <c r="DA16">
         <v>4.8007</v>
@@ -21242,8 +21272,8 @@
       <c r="EG16">
         <v>72.031899999999993</v>
       </c>
-      <c r="EH16">
-        <v>2377900</v>
+      <c r="EH16" t="s">
+        <v>500</v>
       </c>
       <c r="EI16">
         <v>17.786300000000001</v>
@@ -21338,11 +21368,11 @@
       <c r="GN16">
         <v>14.6342</v>
       </c>
-      <c r="GO16">
-        <v>74794117.647100002</v>
-      </c>
-      <c r="HJ16">
-        <v>3709000</v>
+      <c r="GO16" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ16" t="s">
+        <v>500</v>
       </c>
       <c r="HL16">
         <v>11.2403</v>
@@ -21392,8 +21422,8 @@
       <c r="IW16">
         <v>44.729399999999998</v>
       </c>
-      <c r="IY16">
-        <v>34.511899999999997</v>
+      <c r="IY16" t="s">
+        <v>500</v>
       </c>
       <c r="IZ16">
         <v>2.7471999999999999</v>
@@ -21611,8 +21641,8 @@
       <c r="ML16">
         <v>7.7309999999999999</v>
       </c>
-      <c r="MM16">
-        <v>20896213.183699999</v>
+      <c r="MM16" t="s">
+        <v>500</v>
       </c>
       <c r="MN16">
         <v>17.7089</v>
@@ -21719,8 +21749,8 @@
       <c r="OL16">
         <v>8.9855999999999998</v>
       </c>
-      <c r="OM16">
-        <v>2109200</v>
+      <c r="OM16" t="s">
+        <v>500</v>
       </c>
       <c r="OQ16">
         <v>10.885400000000001</v>
@@ -21863,8 +21893,8 @@
       <c r="SD16">
         <v>18.112400000000001</v>
       </c>
-      <c r="SF16">
-        <v>21.328099999999999</v>
+      <c r="SF16" t="s">
+        <v>500</v>
       </c>
       <c r="SG16">
         <v>19.448699999999999</v>
@@ -22135,8 +22165,8 @@
       <c r="CY17">
         <v>2.6783000000000001</v>
       </c>
-      <c r="CZ17">
-        <v>37.5595</v>
+      <c r="CZ17" t="s">
+        <v>500</v>
       </c>
       <c r="DA17">
         <v>1.7941</v>
@@ -22192,8 +22222,8 @@
       <c r="EG17">
         <v>77.638599999999997</v>
       </c>
-      <c r="EH17">
-        <v>2377900</v>
+      <c r="EH17" t="s">
+        <v>500</v>
       </c>
       <c r="EI17">
         <v>19.046600000000002</v>
@@ -22285,11 +22315,11 @@
       <c r="GN17">
         <v>14.648</v>
       </c>
-      <c r="GO17">
-        <v>81588235.294100001</v>
-      </c>
-      <c r="HJ17">
-        <v>2809000</v>
+      <c r="GO17" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ17" t="s">
+        <v>500</v>
       </c>
       <c r="HL17">
         <v>11.914099999999999</v>
@@ -22339,8 +22369,8 @@
       <c r="IW17">
         <v>47.047499999999999</v>
       </c>
-      <c r="IY17">
-        <v>34.511899999999997</v>
+      <c r="IY17" t="s">
+        <v>500</v>
       </c>
       <c r="IZ17">
         <v>2.9872999999999998</v>
@@ -22552,8 +22582,8 @@
       <c r="MK17">
         <v>19.752099999999999</v>
       </c>
-      <c r="MM17">
-        <v>21601683.0295</v>
+      <c r="MM17" t="s">
+        <v>500</v>
       </c>
       <c r="MN17">
         <v>18.155100000000001</v>
@@ -22789,8 +22819,8 @@
       <c r="SD17">
         <v>13.5197</v>
       </c>
-      <c r="SF17">
-        <v>3293260</v>
+      <c r="SF17" t="s">
+        <v>500</v>
       </c>
       <c r="SG17">
         <v>20.743600000000001</v>
@@ -23058,8 +23088,8 @@
       <c r="CY18">
         <v>-0.40849999999999997</v>
       </c>
-      <c r="CZ18">
-        <v>37.5595</v>
+      <c r="CZ18" t="s">
+        <v>500</v>
       </c>
       <c r="DA18">
         <v>0.72929999999999995</v>
@@ -23205,11 +23235,11 @@
       <c r="GN18">
         <v>14.26</v>
       </c>
-      <c r="GO18">
-        <v>74411764.705899999</v>
-      </c>
-      <c r="HJ18">
-        <v>2459620.9553999999</v>
+      <c r="GO18" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ18" t="s">
+        <v>500</v>
       </c>
       <c r="HL18">
         <v>12.8544</v>
@@ -23259,8 +23289,8 @@
       <c r="IW18">
         <v>48.877200000000002</v>
       </c>
-      <c r="IY18">
-        <v>34.511899999999997</v>
+      <c r="IY18" t="s">
+        <v>500</v>
       </c>
       <c r="IZ18">
         <v>3.5920999999999998</v>
@@ -23463,8 +23493,8 @@
       <c r="MK18">
         <v>21.2483</v>
       </c>
-      <c r="MM18">
-        <v>26974789.916000001</v>
+      <c r="MM18" t="s">
+        <v>500</v>
       </c>
       <c r="MN18">
         <v>18.837499999999999</v>
@@ -23490,8 +23520,8 @@
       <c r="MU18">
         <v>8.2611000000000008</v>
       </c>
-      <c r="MV18">
-        <v>47.517299999999999</v>
+      <c r="MV18" t="s">
+        <v>500</v>
       </c>
       <c r="MW18">
         <v>2.9173</v>
@@ -23700,8 +23730,8 @@
       <c r="SD18">
         <v>12.829800000000001</v>
       </c>
-      <c r="SF18">
-        <v>3321130</v>
+      <c r="SF18" t="s">
+        <v>500</v>
       </c>
       <c r="SG18">
         <v>21.400700000000001</v>
@@ -23966,8 +23996,8 @@
       <c r="CY19">
         <v>-0.93710000000000004</v>
       </c>
-      <c r="CZ19">
-        <v>37.5595</v>
+      <c r="CZ19" t="s">
+        <v>500</v>
       </c>
       <c r="DA19">
         <v>2.5097</v>
@@ -24110,11 +24140,11 @@
       <c r="GJ19">
         <v>60.252600000000001</v>
       </c>
-      <c r="GO19">
-        <v>65205882.352899998</v>
-      </c>
-      <c r="HJ19">
-        <v>1921946.3181</v>
+      <c r="GO19" t="s">
+        <v>500</v>
+      </c>
+      <c r="HJ19" t="s">
+        <v>500</v>
       </c>
       <c r="HL19">
         <v>14.103899999999999</v>
@@ -24161,8 +24191,8 @@
       <c r="IW19">
         <v>50.2194</v>
       </c>
-      <c r="IY19">
-        <v>34.511899999999997</v>
+      <c r="IY19" t="s">
+        <v>500</v>
       </c>
       <c r="IZ19">
         <v>4.1548999999999996</v>
@@ -24362,8 +24392,8 @@
       <c r="MK19">
         <v>23.256399999999999</v>
       </c>
-      <c r="MM19">
-        <v>26736694.677900001</v>
+      <c r="MM19" t="s">
+        <v>500</v>
       </c>
       <c r="MN19">
         <v>19.6463</v>
@@ -24593,8 +24623,8 @@
       <c r="SD19">
         <v>16.6906</v>
       </c>
-      <c r="SF19">
-        <v>1033430</v>
+      <c r="SF19" t="s">
+        <v>500</v>
       </c>
       <c r="SG19">
         <v>22.705200000000001</v>
@@ -24856,8 +24886,8 @@
       <c r="CY20">
         <v>-0.1933</v>
       </c>
-      <c r="CZ20">
-        <v>37.5595</v>
+      <c r="CZ20" t="s">
+        <v>500</v>
       </c>
       <c r="DA20">
         <v>2.7991999999999999</v>
@@ -24997,8 +25027,8 @@
       <c r="GJ20">
         <v>62.505299999999998</v>
       </c>
-      <c r="HJ20">
-        <v>1462303.9839000001</v>
+      <c r="HJ20" t="s">
+        <v>500</v>
       </c>
       <c r="HL20">
         <v>13.5649</v>
@@ -25045,8 +25075,8 @@
       <c r="IW20">
         <v>53.024999999999999</v>
       </c>
-      <c r="IY20">
-        <v>34.511899999999997</v>
+      <c r="IY20" t="s">
+        <v>500</v>
       </c>
       <c r="IZ20">
         <v>4.7972999999999999</v>
@@ -25240,8 +25270,8 @@
       <c r="MK20">
         <v>26.576699999999999</v>
       </c>
-      <c r="MM20">
-        <v>26371148.459399998</v>
+      <c r="MM20" t="s">
+        <v>500</v>
       </c>
       <c r="MN20">
         <v>22.681799999999999</v>
@@ -25719,8 +25749,8 @@
       <c r="CY21">
         <v>-0.37769999999999998</v>
       </c>
-      <c r="CZ21">
-        <v>37.5595</v>
+      <c r="CZ21" t="s">
+        <v>500</v>
       </c>
       <c r="DA21">
         <v>2.5221</v>
@@ -25860,8 +25890,8 @@
       <c r="GJ21">
         <v>62.040700000000001</v>
       </c>
-      <c r="HJ21">
-        <v>2047011.7904000001</v>
+      <c r="HJ21" t="s">
+        <v>500</v>
       </c>
       <c r="HL21">
         <v>14.3688</v>
@@ -25908,8 +25938,8 @@
       <c r="IW21">
         <v>56.270400000000002</v>
       </c>
-      <c r="IY21">
-        <v>34.511899999999997</v>
+      <c r="IY21" t="s">
+        <v>500</v>
       </c>
       <c r="IZ21">
         <v>5.9048999999999996</v>
@@ -26103,8 +26133,8 @@
       <c r="MK21">
         <v>29.525700000000001</v>
       </c>
-      <c r="MM21">
-        <v>26948179.271699999</v>
+      <c r="MM21" t="s">
+        <v>500</v>
       </c>
       <c r="MN21">
         <v>23.372699999999998</v>
@@ -26567,8 +26597,8 @@
       <c r="CY22">
         <v>-0.85270000000000001</v>
       </c>
-      <c r="CZ22">
-        <v>37.5595</v>
+      <c r="CZ22" t="s">
+        <v>500</v>
       </c>
       <c r="DA22">
         <v>1.9631000000000001</v>
@@ -26699,8 +26729,8 @@
       <c r="GJ22">
         <v>57.060499999999998</v>
       </c>
-      <c r="HJ22">
-        <v>1494372.0537</v>
+      <c r="HJ22" t="s">
+        <v>500</v>
       </c>
       <c r="HL22">
         <v>15.491400000000001</v>
@@ -26747,8 +26777,8 @@
       <c r="IW22">
         <v>60.725700000000003</v>
       </c>
-      <c r="IY22">
-        <v>155900000</v>
+      <c r="IY22" t="s">
+        <v>500</v>
       </c>
       <c r="IZ22">
         <v>6.9149000000000003</v>
@@ -26840,8 +26870,8 @@
       <c r="KV22">
         <v>46.930399999999999</v>
       </c>
-      <c r="KW22">
-        <v>207.46469999999999</v>
+      <c r="KW22" t="s">
+        <v>500</v>
       </c>
       <c r="KX22">
         <v>-1.7085999999999999</v>
@@ -26936,8 +26966,8 @@
       <c r="MK22">
         <v>35.330500000000001</v>
       </c>
-      <c r="MM22">
-        <v>23796918.767499998</v>
+      <c r="MM22" t="s">
+        <v>500</v>
       </c>
       <c r="MN22">
         <v>25.317799999999998</v>
@@ -27400,8 +27430,8 @@
       <c r="CY23">
         <v>0.75519999999999998</v>
       </c>
-      <c r="CZ23">
-        <v>37.5595</v>
+      <c r="CZ23" t="s">
+        <v>500</v>
       </c>
       <c r="DA23">
         <v>2.1154999999999999</v>
@@ -27526,8 +27556,8 @@
       <c r="GJ23">
         <v>61.83</v>
       </c>
-      <c r="HJ23">
-        <v>1451614.6273000001</v>
+      <c r="HJ23" t="s">
+        <v>500</v>
       </c>
       <c r="HL23">
         <v>16.4803</v>
@@ -27571,8 +27601,8 @@
       <c r="IW23">
         <v>64.122200000000007</v>
       </c>
-      <c r="IY23">
-        <v>162370000</v>
+      <c r="IY23" t="s">
+        <v>500</v>
       </c>
       <c r="IZ23">
         <v>6.16</v>
@@ -27661,8 +27691,8 @@
       <c r="KV23">
         <v>49.7209</v>
       </c>
-      <c r="KW23">
-        <v>259.52679999999998</v>
+      <c r="KW23" t="s">
+        <v>500</v>
       </c>
       <c r="KX23">
         <v>-1.5109999999999999</v>
@@ -27757,8 +27787,8 @@
       <c r="MK23">
         <v>29.441700000000001</v>
       </c>
-      <c r="MM23">
-        <v>23845938.375399999</v>
+      <c r="MM23" t="s">
+        <v>500</v>
       </c>
       <c r="MN23">
         <v>33.325800000000001</v>
@@ -28200,8 +28230,8 @@
       <c r="CY24">
         <v>-0.74209999999999998</v>
       </c>
-      <c r="CZ24">
-        <v>37.5595</v>
+      <c r="CZ24" t="s">
+        <v>500</v>
       </c>
       <c r="DA24">
         <v>8.4314999999999998</v>
@@ -28317,8 +28347,8 @@
       <c r="GE24">
         <v>9.3727999999999998</v>
       </c>
-      <c r="HJ24">
-        <v>1778708.9395000001</v>
+      <c r="HJ24" t="s">
+        <v>500</v>
       </c>
       <c r="HL24">
         <v>16.7121</v>
@@ -28362,8 +28392,8 @@
       <c r="IW24">
         <v>44.929600000000001</v>
       </c>
-      <c r="IY24">
-        <v>171450000</v>
+      <c r="IY24" t="s">
+        <v>500</v>
       </c>
       <c r="IZ24">
         <v>6.8061999999999996</v>
@@ -28530,8 +28560,8 @@
       <c r="MK24">
         <v>31.5123</v>
       </c>
-      <c r="MM24">
-        <v>22093837.535</v>
+      <c r="MM24" t="s">
+        <v>500</v>
       </c>
       <c r="MN24">
         <v>56.568300000000001</v>

</xml_diff>